<commit_message>
Edited visualizer.py and gantt chart
</commit_message>
<xml_diff>
--- a/Documentation/gantt_chart.xlsx
+++ b/Documentation/gantt_chart.xlsx
@@ -3,13 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{B273D614-6D80-4E11-9500-A63E2907A499}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB5687AA-0D20-4F0D-9A7C-0FAD24D1FC8A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectSchedule" sheetId="11" r:id="rId1"/>
-    <sheet name="About" sheetId="12" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="Display_Week">ProjectSchedule!$E$4</definedName>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="48">
   <si>
     <t>Task 3</t>
   </si>
@@ -44,9 +43,6 @@
   </si>
   <si>
     <t>Task 5</t>
-  </si>
-  <si>
-    <t>Task 1</t>
   </si>
   <si>
     <t>Task 2</t>
@@ -65,9 +61,6 @@
 TO</t>
   </si>
   <si>
-    <t>Project Management Templates</t>
-  </si>
-  <si>
     <t>START</t>
   </si>
   <si>
@@ -83,60 +76,16 @@
     <t>TASK</t>
   </si>
   <si>
-    <t>More Project Management Templates</t>
-  </si>
-  <si>
-    <t>About This Template</t>
-  </si>
-  <si>
     <t>SIMPLE GANTT CHART by Vertex42.com</t>
   </si>
   <si>
-    <t>Additional Help</t>
-  </si>
-  <si>
-    <t>About Vertex42</t>
-  </si>
-  <si>
-    <t>Vertex42.com provides over 300 professionally designed spreadsheet templates for business, home, and education - most of which are free to download. Their collection includes a variety of calendars, planners, and schedules as well as personal finance spreadsheets for budgeting, debt reduction, and loan amortization.</t>
-  </si>
-  <si>
-    <t>Businesses will find invoices, time sheets, inventory trackers, financial statements, and project planning templates. Teachers and students will find resources such as class schedules, grade books, and attendance sheets. Organize your family life with meal planners, checklists, and exercise logs. Each template is thoroughly researched, refined, and improved over time through feedback from thousands of users.</t>
-  </si>
-  <si>
     <t>https://www.vertex42.com/ExcelTemplates/simple-gantt-chart.html</t>
   </si>
   <si>
-    <t>Visit Vertex42.com to download other project management templates, including different types of project schedules, Gantt charts, tasks lists, etc.</t>
-  </si>
-  <si>
-    <t>How to Use the Simple Gantt Chart</t>
-  </si>
-  <si>
-    <t>This template provides a simple way to create a Gantt chart to help visualize and track your project. Simply enter your tasks and start and end dates - no formulas required. The bars in the Gantt chart represent the duration of the task and are displayed using conditional formatting. Insert new tasks by inserting new rows.</t>
-  </si>
-  <si>
-    <t>Click on the link below to visit vertex42.com and learn more about how to use this template, such as how to calculate days and work days, create task dependencies, change the colors of the bars, add a scroll bar to make it easier to change the display week, extend the date range displayed in the chart, etc.</t>
-  </si>
-  <si>
-    <t>There are 2 worksheets in this workbook. 
-TimeSheet
-About
-The instructions for each worksheet are in the A column starting in cell A1 of each worksheet. They are written with hidden text. Each step guides you through the information in that row. Each subsequent step continues in cell A2, A3, and so on, unless otherwise explicitly directed. For example, instruction text might say "continue to cell A6" for the next step. 
-This hidden text will not print.
-To remove these instructions from the worksheet, simply delete column A.</t>
-  </si>
-  <si>
-    <t>Guide for Screen Readers</t>
-  </si>
-  <si>
     <t>Enter Company Name in cell B2.</t>
   </si>
   <si>
     <t>date</t>
-  </si>
-  <si>
-    <t>Name</t>
   </si>
   <si>
     <t>Sample phase title block</t>
@@ -221,12 +170,6 @@
     <t>Bringing the model together</t>
   </si>
   <si>
-    <t>Run Package for Multiple Routes</t>
-  </si>
-  <si>
-    <t>Create Database</t>
-  </si>
-  <si>
     <t>Set up repository in Shablohna format</t>
   </si>
   <si>
@@ -248,9 +191,6 @@
     <t>Real-time data tech review</t>
   </si>
   <si>
-    <t>Route_dynamics (GIS) bug fixes</t>
-  </si>
-  <si>
     <t>Combine import functions into one notebook</t>
   </si>
   <si>
@@ -260,7 +200,19 @@
     <t>Add vehicle dynamics equations</t>
   </si>
   <si>
-    <t>Interpolate between elevation points</t>
+    <t>All</t>
+  </si>
+  <si>
+    <t>Erica</t>
+  </si>
+  <si>
+    <t>Presentation</t>
+  </si>
+  <si>
+    <t>Poster</t>
+  </si>
+  <si>
+    <t>Ryan and Erica</t>
   </si>
 </sst>
 </file>
@@ -274,7 +226,7 @@
     <numFmt numFmtId="166" formatCode="mmm\ d\,\ yyyy"/>
     <numFmt numFmtId="167" formatCode="d"/>
   </numFmts>
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -390,64 +342,14 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1" tint="0.34998626667073579"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1" tint="0.499984740745262"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="20"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="major"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF1D2129"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="16"/>
-      <color theme="4" tint="-0.249977111117893"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="major"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="16">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -524,18 +426,6 @@
       <patternFill patternType="solid">
         <fgColor theme="1" tint="0.34998626667073579"/>
         <bgColor theme="4"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -667,7 +557,7 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="9" fillId="0" borderId="3" applyFont="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -690,7 +580,7 @@
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -824,39 +714,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="3" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1" applyProtection="1">
@@ -887,9 +749,6 @@
     <xf numFmtId="0" fontId="9" fillId="8" borderId="2" xfId="11" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="11" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="9" borderId="2" xfId="11" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -907,9 +766,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="10" borderId="2" xfId="11" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="12" applyFill="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="12" applyFill="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
@@ -920,6 +776,30 @@
     <xf numFmtId="0" fontId="9" fillId="10" borderId="2" xfId="12" applyFill="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="12" applyFont="1" applyFill="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="11" applyFont="1" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="12" applyFont="1" applyFill="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="12" applyFont="1" applyFill="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="3" xfId="9">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="8">
       <alignment horizontal="right" indent="1"/>
     </xf>
@@ -927,69 +807,14 @@
       <alignment horizontal="right" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="3" xfId="9">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="2" xfId="11" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="14" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="14" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="14" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="3" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="15" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="15" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="2" xfId="11" applyFont="1" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="12" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="11" applyFont="1" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="12" applyFont="1" applyFill="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="11" applyFont="1" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="12" applyFont="1" applyFill="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="12" applyFont="1" applyFill="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="11" applyFont="1" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -1007,37 +832,7 @@
     <cellStyle name="Title" xfId="5" builtinId="15" customBuiltin="1"/>
     <cellStyle name="zHiddenText" xfId="3" xr:uid="{26E66EE6-E33F-4D77-BAE4-0FB4F5BBF673}"/>
   </cellStyles>
-  <dxfs count="15">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
+  <dxfs count="12">
     <dxf>
       <fill>
         <patternFill>
@@ -1164,15 +959,15 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="ToDoList" pivot="0" count="9" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="14"/>
-      <tableStyleElement type="headerRow" dxfId="13"/>
-      <tableStyleElement type="totalRow" dxfId="12"/>
-      <tableStyleElement type="firstColumn" dxfId="11"/>
-      <tableStyleElement type="lastColumn" dxfId="10"/>
-      <tableStyleElement type="firstRowStripe" dxfId="9"/>
-      <tableStyleElement type="secondRowStripe" dxfId="8"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="7"/>
-      <tableStyleElement type="secondColumnStripe" dxfId="6"/>
+      <tableStyleElement type="wholeTable" dxfId="11"/>
+      <tableStyleElement type="headerRow" dxfId="10"/>
+      <tableStyleElement type="totalRow" dxfId="9"/>
+      <tableStyleElement type="firstColumn" dxfId="8"/>
+      <tableStyleElement type="lastColumn" dxfId="7"/>
+      <tableStyleElement type="firstRowStripe" dxfId="6"/>
+      <tableStyleElement type="secondRowStripe" dxfId="5"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="4"/>
+      <tableStyleElement type="secondColumnStripe" dxfId="3"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -1263,62 +1058,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>1905000</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>523875</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1" descr="Vertex42 logo">
-          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8638EF3-2DAE-40BC-A45A-2B8C536FAB0D}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="190500" y="95250"/>
-          <a:ext cx="1905000" cy="428625"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1587,16 +1326,16 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:CM37"/>
+  <dimension ref="A1:BL32"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="B1" zoomScale="103" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B19" sqref="B19"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="103" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="BF4" sqref="BF4:BL4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="2.7265625" style="57" customWidth="1"/>
+    <col min="1" max="1" width="2.7265625" style="47" customWidth="1"/>
     <col min="2" max="2" width="36.90625" customWidth="1"/>
     <col min="3" max="3" width="14.08984375" customWidth="1"/>
     <col min="4" max="4" width="10.7265625" customWidth="1"/>
@@ -1609,11 +1348,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="A1" s="58" t="s">
-        <v>35</v>
-      </c>
-      <c r="B1" s="62" t="s">
-        <v>44</v>
+      <c r="A1" s="48" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="52" t="s">
+        <v>29</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="2"/>
@@ -1621,134 +1360,134 @@
       <c r="F1" s="46"/>
       <c r="H1" s="2"/>
       <c r="I1" s="14" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="57" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" s="63"/>
-      <c r="I2" s="60" t="s">
-        <v>22</v>
+      <c r="A2" s="47" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="53"/>
+      <c r="I2" s="50" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="57" t="s">
-        <v>36</v>
-      </c>
-      <c r="B3" s="64"/>
-      <c r="C3" s="81" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="82"/>
-      <c r="E3" s="87">
+      <c r="A3" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="54"/>
+      <c r="C3" s="77" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="78"/>
+      <c r="E3" s="76">
         <v>43565</v>
       </c>
-      <c r="F3" s="87"/>
+      <c r="F3" s="76"/>
     </row>
     <row r="4" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="58" t="s">
-        <v>37</v>
-      </c>
-      <c r="C4" s="81" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="82"/>
+      <c r="A4" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="77" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="78"/>
       <c r="E4" s="7">
         <v>1</v>
       </c>
-      <c r="I4" s="84">
+      <c r="I4" s="73">
         <f>I5</f>
         <v>43563</v>
       </c>
-      <c r="J4" s="85"/>
-      <c r="K4" s="85"/>
-      <c r="L4" s="85"/>
-      <c r="M4" s="85"/>
-      <c r="N4" s="85"/>
-      <c r="O4" s="86"/>
-      <c r="P4" s="84">
+      <c r="J4" s="74"/>
+      <c r="K4" s="74"/>
+      <c r="L4" s="74"/>
+      <c r="M4" s="74"/>
+      <c r="N4" s="74"/>
+      <c r="O4" s="75"/>
+      <c r="P4" s="73">
         <f>P5</f>
         <v>43570</v>
       </c>
-      <c r="Q4" s="85"/>
-      <c r="R4" s="85"/>
-      <c r="S4" s="85"/>
-      <c r="T4" s="85"/>
-      <c r="U4" s="85"/>
-      <c r="V4" s="86"/>
-      <c r="W4" s="84">
+      <c r="Q4" s="74"/>
+      <c r="R4" s="74"/>
+      <c r="S4" s="74"/>
+      <c r="T4" s="74"/>
+      <c r="U4" s="74"/>
+      <c r="V4" s="75"/>
+      <c r="W4" s="73">
         <f>W5</f>
         <v>43577</v>
       </c>
-      <c r="X4" s="85"/>
-      <c r="Y4" s="85"/>
-      <c r="Z4" s="85"/>
-      <c r="AA4" s="85"/>
-      <c r="AB4" s="85"/>
-      <c r="AC4" s="86"/>
-      <c r="AD4" s="84">
+      <c r="X4" s="74"/>
+      <c r="Y4" s="74"/>
+      <c r="Z4" s="74"/>
+      <c r="AA4" s="74"/>
+      <c r="AB4" s="74"/>
+      <c r="AC4" s="75"/>
+      <c r="AD4" s="73">
         <f>AD5</f>
         <v>43584</v>
       </c>
-      <c r="AE4" s="85"/>
-      <c r="AF4" s="85"/>
-      <c r="AG4" s="85"/>
-      <c r="AH4" s="85"/>
-      <c r="AI4" s="85"/>
-      <c r="AJ4" s="86"/>
-      <c r="AK4" s="84">
+      <c r="AE4" s="74"/>
+      <c r="AF4" s="74"/>
+      <c r="AG4" s="74"/>
+      <c r="AH4" s="74"/>
+      <c r="AI4" s="74"/>
+      <c r="AJ4" s="75"/>
+      <c r="AK4" s="73">
         <f>AK5</f>
         <v>43591</v>
       </c>
-      <c r="AL4" s="85"/>
-      <c r="AM4" s="85"/>
-      <c r="AN4" s="85"/>
-      <c r="AO4" s="85"/>
-      <c r="AP4" s="85"/>
-      <c r="AQ4" s="86"/>
-      <c r="AR4" s="84">
+      <c r="AL4" s="74"/>
+      <c r="AM4" s="74"/>
+      <c r="AN4" s="74"/>
+      <c r="AO4" s="74"/>
+      <c r="AP4" s="74"/>
+      <c r="AQ4" s="75"/>
+      <c r="AR4" s="73">
         <f>AR5</f>
         <v>43598</v>
       </c>
-      <c r="AS4" s="85"/>
-      <c r="AT4" s="85"/>
-      <c r="AU4" s="85"/>
-      <c r="AV4" s="85"/>
-      <c r="AW4" s="85"/>
-      <c r="AX4" s="86"/>
-      <c r="AY4" s="84">
+      <c r="AS4" s="74"/>
+      <c r="AT4" s="74"/>
+      <c r="AU4" s="74"/>
+      <c r="AV4" s="74"/>
+      <c r="AW4" s="74"/>
+      <c r="AX4" s="75"/>
+      <c r="AY4" s="73">
         <f>AY5</f>
         <v>43605</v>
       </c>
-      <c r="AZ4" s="85"/>
-      <c r="BA4" s="85"/>
-      <c r="BB4" s="85"/>
-      <c r="BC4" s="85"/>
-      <c r="BD4" s="85"/>
-      <c r="BE4" s="86"/>
-      <c r="BF4" s="84">
+      <c r="AZ4" s="74"/>
+      <c r="BA4" s="74"/>
+      <c r="BB4" s="74"/>
+      <c r="BC4" s="74"/>
+      <c r="BD4" s="74"/>
+      <c r="BE4" s="75"/>
+      <c r="BF4" s="73">
         <f>BF5</f>
         <v>43612</v>
       </c>
-      <c r="BG4" s="85"/>
-      <c r="BH4" s="85"/>
-      <c r="BI4" s="85"/>
-      <c r="BJ4" s="85"/>
-      <c r="BK4" s="85"/>
-      <c r="BL4" s="86"/>
+      <c r="BG4" s="74"/>
+      <c r="BH4" s="74"/>
+      <c r="BI4" s="74"/>
+      <c r="BJ4" s="74"/>
+      <c r="BK4" s="74"/>
+      <c r="BL4" s="75"/>
     </row>
     <row r="5" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="58" t="s">
-        <v>38</v>
-      </c>
-      <c r="B5" s="83"/>
-      <c r="C5" s="83"/>
-      <c r="D5" s="83"/>
-      <c r="E5" s="83"/>
-      <c r="F5" s="83"/>
-      <c r="G5" s="83"/>
+      <c r="A5" s="48" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="79"/>
+      <c r="C5" s="79"/>
+      <c r="D5" s="79"/>
+      <c r="E5" s="79"/>
+      <c r="F5" s="79"/>
+      <c r="G5" s="79"/>
       <c r="I5" s="11">
         <f>Project_Start-WEEKDAY(Project_Start,1)+2+7*(Display_Week-1)</f>
         <v>43563</v>
@@ -1975,27 +1714,27 @@
       </c>
     </row>
     <row r="6" spans="1:64" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="58" t="s">
-        <v>39</v>
+      <c r="A6" s="48" t="s">
+        <v>24</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C6" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>10</v>
-      </c>
       <c r="F6" s="9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G6" s="9"/>
       <c r="H6" s="9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I6" s="13" t="str">
         <f t="shared" ref="I6" si="3">LEFT(TEXT(I5,"ddd"),1)</f>
@@ -2223,10 +1962,10 @@
       </c>
     </row>
     <row r="7" spans="1:64" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="57" t="s">
-        <v>34</v>
-      </c>
-      <c r="C7" s="61"/>
+      <c r="A7" s="47" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="51"/>
       <c r="E7"/>
       <c r="H7" t="str">
         <f>IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
@@ -2290,19 +2029,19 @@
       <c r="BL7" s="43"/>
     </row>
     <row r="8" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="58" t="s">
-        <v>40</v>
+      <c r="A8" s="48" t="s">
+        <v>25</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="C8" s="69"/>
+        <v>30</v>
+      </c>
+      <c r="C8" s="59"/>
       <c r="D8" s="18"/>
       <c r="E8" s="19"/>
       <c r="F8" s="20"/>
       <c r="G8" s="16"/>
       <c r="H8" s="16" t="str">
-        <f t="shared" ref="H8:H34" si="6">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
+        <f t="shared" ref="H8:H29" si="6">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v/>
       </c>
       <c r="I8" s="43"/>
@@ -2363,22 +2102,22 @@
       <c r="BL8" s="43"/>
     </row>
     <row r="9" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="58" t="s">
-        <v>41</v>
-      </c>
-      <c r="B9" s="100" t="s">
-        <v>50</v>
+      <c r="A9" s="48" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="69" t="s">
+        <v>33</v>
       </c>
       <c r="C9" s="70" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="D9" s="21">
-        <v>0</v>
-      </c>
-      <c r="E9" s="65">
+        <v>1</v>
+      </c>
+      <c r="E9" s="55">
         <v>43566</v>
       </c>
-      <c r="F9" s="65">
+      <c r="F9" s="55">
         <f>E9+3</f>
         <v>43569</v>
       </c>
@@ -2445,22 +2184,22 @@
       <c r="BL9" s="43"/>
     </row>
     <row r="10" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="58" t="s">
-        <v>42</v>
-      </c>
-      <c r="B10" s="100" t="s">
-        <v>51</v>
-      </c>
-      <c r="C10" s="101" t="s">
-        <v>52</v>
+      <c r="A10" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="69" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="70" t="s">
+        <v>35</v>
       </c>
       <c r="D10" s="21">
-        <v>0.5</v>
-      </c>
-      <c r="E10" s="65">
+        <v>1</v>
+      </c>
+      <c r="E10" s="55">
         <v>43563</v>
       </c>
-      <c r="F10" s="65">
+      <c r="F10" s="55">
         <f>E10+7</f>
         <v>43570</v>
       </c>
@@ -2527,20 +2266,20 @@
       <c r="BL10" s="43"/>
     </row>
     <row r="11" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="57"/>
-      <c r="B11" s="100" t="s">
-        <v>53</v>
-      </c>
-      <c r="C11" s="101" t="s">
-        <v>52</v>
+      <c r="A11" s="47"/>
+      <c r="B11" s="69" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="70" t="s">
+        <v>35</v>
       </c>
       <c r="D11" s="21">
-        <v>0.5</v>
-      </c>
-      <c r="E11" s="65">
+        <v>1</v>
+      </c>
+      <c r="E11" s="55">
         <v>43563</v>
       </c>
-      <c r="F11" s="65">
+      <c r="F11" s="55">
         <f>E11+7</f>
         <v>43570</v>
       </c>
@@ -2607,18 +2346,20 @@
       <c r="BL11" s="43"/>
     </row>
     <row r="12" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="57"/>
-      <c r="B12" s="100" t="s">
-        <v>54</v>
-      </c>
-      <c r="C12" s="70"/>
+      <c r="A12" s="47"/>
+      <c r="B12" s="69" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="70" t="s">
+        <v>43</v>
+      </c>
       <c r="D12" s="21">
         <v>1</v>
       </c>
-      <c r="E12" s="65">
+      <c r="E12" s="55">
         <v>43563</v>
       </c>
-      <c r="F12" s="65">
+      <c r="F12" s="55">
         <f>E12+2</f>
         <v>43565</v>
       </c>
@@ -2685,24 +2426,20 @@
       <c r="BL12" s="43"/>
     </row>
     <row r="13" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="57"/>
-      <c r="B13" s="77" t="s">
-        <v>2</v>
-      </c>
-      <c r="C13" s="70"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="65">
-        <f>E10+1</f>
-        <v>43564</v>
-      </c>
-      <c r="F13" s="65">
-        <f>E13+2</f>
-        <v>43566</v>
-      </c>
+      <c r="A13" s="48" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="60"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="25"/>
       <c r="G13" s="16"/>
-      <c r="H13" s="16">
+      <c r="H13" s="16" t="str">
         <f t="shared" si="6"/>
-        <v>3</v>
+        <v/>
       </c>
       <c r="I13" s="43"/>
       <c r="J13" s="43"/>
@@ -2762,20 +2499,25 @@
       <c r="BL13" s="43"/>
     </row>
     <row r="14" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="58" t="s">
-        <v>43</v>
-      </c>
-      <c r="B14" s="22" t="s">
-        <v>46</v>
-      </c>
-      <c r="C14" s="71"/>
-      <c r="D14" s="23"/>
-      <c r="E14" s="24"/>
-      <c r="F14" s="25"/>
+      <c r="A14" s="48"/>
+      <c r="B14" s="71" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="61"/>
+      <c r="D14" s="26">
+        <v>1</v>
+      </c>
+      <c r="E14" s="56">
+        <v>43572</v>
+      </c>
+      <c r="F14" s="56">
+        <f>E14+4</f>
+        <v>43576</v>
+      </c>
       <c r="G14" s="16"/>
-      <c r="H14" s="16" t="str">
+      <c r="H14" s="16">
         <f t="shared" si="6"/>
-        <v/>
+        <v>5</v>
       </c>
       <c r="I14" s="43"/>
       <c r="J14" s="43"/>
@@ -2835,25 +2577,27 @@
       <c r="BL14" s="43"/>
     </row>
     <row r="15" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="58"/>
-      <c r="B15" s="102" t="s">
-        <v>55</v>
-      </c>
-      <c r="C15" s="72"/>
+      <c r="A15" s="47"/>
+      <c r="B15" s="71" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" s="80" t="s">
+        <v>44</v>
+      </c>
       <c r="D15" s="26">
-        <v>0</v>
-      </c>
-      <c r="E15" s="66">
+        <v>1</v>
+      </c>
+      <c r="E15" s="56">
         <v>43572</v>
       </c>
-      <c r="F15" s="66">
-        <f>E15+4</f>
-        <v>43576</v>
+      <c r="F15" s="56">
+        <f>E15+5</f>
+        <v>43577</v>
       </c>
       <c r="G15" s="16"/>
       <c r="H15" s="16">
         <f t="shared" si="6"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I15" s="43"/>
       <c r="J15" s="43"/>
@@ -2867,8 +2611,8 @@
       <c r="R15" s="43"/>
       <c r="S15" s="43"/>
       <c r="T15" s="43"/>
-      <c r="U15" s="43"/>
-      <c r="V15" s="43"/>
+      <c r="U15" s="44"/>
+      <c r="V15" s="44"/>
       <c r="W15" s="43"/>
       <c r="X15" s="43"/>
       <c r="Y15" s="43"/>
@@ -2913,25 +2657,24 @@
       <c r="BL15" s="43"/>
     </row>
     <row r="16" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="57"/>
-      <c r="B16" s="102" t="s">
-        <v>56</v>
-      </c>
-      <c r="C16" s="72"/>
-      <c r="D16" s="26">
-        <v>0</v>
-      </c>
-      <c r="E16" s="66">
-        <v>43572</v>
-      </c>
-      <c r="F16" s="66">
-        <f>E16+5</f>
-        <v>43577</v>
+      <c r="A16" s="47"/>
+      <c r="B16" s="66" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" s="61"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="56" t="e">
+        <f>#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="F16" s="56" t="e">
+        <f>E16+3</f>
+        <v>#REF!</v>
       </c>
       <c r="G16" s="16"/>
-      <c r="H16" s="16">
+      <c r="H16" s="16" t="e">
         <f t="shared" si="6"/>
-        <v>6</v>
+        <v>#REF!</v>
       </c>
       <c r="I16" s="43"/>
       <c r="J16" s="43"/>
@@ -2945,8 +2688,8 @@
       <c r="R16" s="43"/>
       <c r="S16" s="43"/>
       <c r="T16" s="43"/>
-      <c r="U16" s="44"/>
-      <c r="V16" s="44"/>
+      <c r="U16" s="43"/>
+      <c r="V16" s="43"/>
       <c r="W16" s="43"/>
       <c r="X16" s="43"/>
       <c r="Y16" s="43"/>
@@ -2990,24 +2733,21 @@
       <c r="BK16" s="43"/>
       <c r="BL16" s="43"/>
     </row>
-    <row r="17" spans="1:91" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="57"/>
-      <c r="B17" s="102" t="s">
-        <v>57</v>
-      </c>
-      <c r="C17" s="72"/>
-      <c r="D17" s="26"/>
-      <c r="E17" s="66">
-        <v>43575</v>
-      </c>
-      <c r="F17" s="66">
-        <f>E17+3</f>
-        <v>43578</v>
-      </c>
+    <row r="17" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="62"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="30"/>
       <c r="G17" s="16"/>
-      <c r="H17" s="16">
+      <c r="H17" s="16" t="str">
         <f t="shared" si="6"/>
-        <v>4</v>
+        <v/>
       </c>
       <c r="I17" s="43"/>
       <c r="J17" s="43"/>
@@ -3066,25 +2806,25 @@
       <c r="BK17" s="43"/>
       <c r="BL17" s="43"/>
     </row>
-    <row r="18" spans="1:91" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="57"/>
-      <c r="B18" s="102" t="s">
-        <v>61</v>
-      </c>
-      <c r="C18" s="72"/>
-      <c r="D18" s="26"/>
-      <c r="E18" s="66">
-        <f>E17</f>
-        <v>43575</v>
-      </c>
-      <c r="F18" s="66">
-        <f>E18+2</f>
-        <v>43577</v>
+    <row r="18" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="47"/>
+      <c r="B18" s="72" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" s="63"/>
+      <c r="D18" s="31"/>
+      <c r="E18" s="57">
+        <f>E9+15</f>
+        <v>43581</v>
+      </c>
+      <c r="F18" s="57">
+        <f>E18+5</f>
+        <v>43586</v>
       </c>
       <c r="G18" s="16"/>
       <c r="H18" s="16">
         <f t="shared" si="6"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I18" s="43"/>
       <c r="J18" s="43"/>
@@ -3102,7 +2842,7 @@
       <c r="V18" s="43"/>
       <c r="W18" s="43"/>
       <c r="X18" s="43"/>
-      <c r="Y18" s="44"/>
+      <c r="Y18" s="43"/>
       <c r="Z18" s="43"/>
       <c r="AA18" s="43"/>
       <c r="AB18" s="43"/>
@@ -3143,25 +2883,25 @@
       <c r="BK18" s="43"/>
       <c r="BL18" s="43"/>
     </row>
-    <row r="19" spans="1:91" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="57"/>
-      <c r="B19" s="78" t="s">
-        <v>2</v>
-      </c>
-      <c r="C19" s="72"/>
-      <c r="D19" s="26"/>
-      <c r="E19" s="66">
-        <f>E18</f>
-        <v>43575</v>
-      </c>
-      <c r="F19" s="66">
-        <f>E19+3</f>
-        <v>43578</v>
+    <row r="19" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="47"/>
+      <c r="B19" s="72" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" s="63"/>
+      <c r="D19" s="31"/>
+      <c r="E19" s="57">
+        <f>F18+1</f>
+        <v>43587</v>
+      </c>
+      <c r="F19" s="57">
+        <f>E19+4</f>
+        <v>43591</v>
       </c>
       <c r="G19" s="16"/>
       <c r="H19" s="16">
         <f t="shared" si="6"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I19" s="43"/>
       <c r="J19" s="43"/>
@@ -3220,21 +2960,25 @@
       <c r="BK19" s="43"/>
       <c r="BL19" s="43"/>
     </row>
-    <row r="20" spans="1:91" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="57" t="s">
-        <v>32</v>
-      </c>
-      <c r="B20" s="27" t="s">
-        <v>47</v>
-      </c>
-      <c r="C20" s="73"/>
-      <c r="D20" s="28"/>
-      <c r="E20" s="29"/>
-      <c r="F20" s="30"/>
+    <row r="20" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="47"/>
+      <c r="B20" s="72" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" s="63"/>
+      <c r="D20" s="31"/>
+      <c r="E20" s="57">
+        <f>E19+5</f>
+        <v>43592</v>
+      </c>
+      <c r="F20" s="57">
+        <f>E20+5</f>
+        <v>43597</v>
+      </c>
       <c r="G20" s="16"/>
-      <c r="H20" s="16" t="str">
+      <c r="H20" s="16">
         <f t="shared" si="6"/>
-        <v/>
+        <v>6</v>
       </c>
       <c r="I20" s="43"/>
       <c r="J20" s="43"/>
@@ -3293,25 +3037,25 @@
       <c r="BK20" s="43"/>
       <c r="BL20" s="43"/>
     </row>
-    <row r="21" spans="1:91" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="57"/>
-      <c r="B21" s="105" t="s">
-        <v>58</v>
-      </c>
-      <c r="C21" s="74"/>
+    <row r="21" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="47"/>
+      <c r="B21" s="67" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="63"/>
       <c r="D21" s="31"/>
-      <c r="E21" s="67">
-        <f>E9+15</f>
-        <v>43581</v>
-      </c>
-      <c r="F21" s="67">
-        <f>E21+5</f>
-        <v>43586</v>
+      <c r="E21" s="57">
+        <f>F20+1</f>
+        <v>43598</v>
+      </c>
+      <c r="F21" s="57">
+        <f>E21+4</f>
+        <v>43602</v>
       </c>
       <c r="G21" s="16"/>
       <c r="H21" s="16">
         <f t="shared" si="6"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I21" s="43"/>
       <c r="J21" s="43"/>
@@ -3370,20 +3114,20 @@
       <c r="BK21" s="43"/>
       <c r="BL21" s="43"/>
     </row>
-    <row r="22" spans="1:91" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="57"/>
-      <c r="B22" s="105" t="s">
-        <v>59</v>
-      </c>
-      <c r="C22" s="74"/>
+    <row r="22" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="47"/>
+      <c r="B22" s="67" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" s="63"/>
       <c r="D22" s="31"/>
-      <c r="E22" s="67">
-        <f>F21+1</f>
-        <v>43587</v>
-      </c>
-      <c r="F22" s="67">
+      <c r="E22" s="57">
+        <f>E20</f>
+        <v>43592</v>
+      </c>
+      <c r="F22" s="57">
         <f>E22+4</f>
-        <v>43591</v>
+        <v>43596</v>
       </c>
       <c r="G22" s="16"/>
       <c r="H22" s="16">
@@ -3447,25 +3191,21 @@
       <c r="BK22" s="43"/>
       <c r="BL22" s="43"/>
     </row>
-    <row r="23" spans="1:91" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="57"/>
-      <c r="B23" s="105" t="s">
-        <v>60</v>
-      </c>
-      <c r="C23" s="74"/>
-      <c r="D23" s="31"/>
-      <c r="E23" s="67">
-        <f>E22+5</f>
-        <v>43592</v>
-      </c>
-      <c r="F23" s="67">
-        <f>E23+5</f>
-        <v>43597</v>
-      </c>
+    <row r="23" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="B23" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="C23" s="64"/>
+      <c r="D23" s="33"/>
+      <c r="E23" s="34"/>
+      <c r="F23" s="35"/>
       <c r="G23" s="16"/>
-      <c r="H23" s="16">
+      <c r="H23" s="16" t="str">
         <f t="shared" si="6"/>
-        <v>6</v>
+        <v/>
       </c>
       <c r="I23" s="43"/>
       <c r="J23" s="43"/>
@@ -3524,25 +3264,25 @@
       <c r="BK23" s="43"/>
       <c r="BL23" s="43"/>
     </row>
-    <row r="24" spans="1:91" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A24" s="57"/>
-      <c r="B24" s="79" t="s">
-        <v>1</v>
-      </c>
-      <c r="C24" s="74"/>
-      <c r="D24" s="31"/>
-      <c r="E24" s="67">
-        <f>F23+1</f>
-        <v>43598</v>
-      </c>
-      <c r="F24" s="67">
-        <f>E24+4</f>
-        <v>43602</v>
+    <row r="24" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A24" s="47"/>
+      <c r="B24" s="81" t="s">
+        <v>46</v>
+      </c>
+      <c r="C24" s="82" t="s">
+        <v>47</v>
+      </c>
+      <c r="D24" s="36"/>
+      <c r="E24" s="58">
+        <v>43626</v>
+      </c>
+      <c r="F24" s="58">
+        <v>43636</v>
       </c>
       <c r="G24" s="16"/>
       <c r="H24" s="16">
         <f t="shared" si="6"/>
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="I24" s="43"/>
       <c r="J24" s="43"/>
@@ -3601,25 +3341,23 @@
       <c r="BK24" s="43"/>
       <c r="BL24" s="43"/>
     </row>
-    <row r="25" spans="1:91" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="57"/>
-      <c r="B25" s="79" t="s">
-        <v>2</v>
-      </c>
-      <c r="C25" s="74"/>
-      <c r="D25" s="31"/>
-      <c r="E25" s="67">
-        <f>E23</f>
-        <v>43592</v>
-      </c>
-      <c r="F25" s="67">
-        <f>E25+4</f>
-        <v>43596</v>
+    <row r="25" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A25" s="47"/>
+      <c r="B25" s="68" t="s">
+        <v>3</v>
+      </c>
+      <c r="C25" s="65"/>
+      <c r="D25" s="36"/>
+      <c r="E25" s="58" t="s">
+        <v>16</v>
+      </c>
+      <c r="F25" s="58" t="s">
+        <v>16</v>
       </c>
       <c r="G25" s="16"/>
-      <c r="H25" s="16">
+      <c r="H25" s="16" t="e">
         <f t="shared" si="6"/>
-        <v>5</v>
+        <v>#VALUE!</v>
       </c>
       <c r="I25" s="43"/>
       <c r="J25" s="43"/>
@@ -3678,21 +3416,23 @@
       <c r="BK25" s="43"/>
       <c r="BL25" s="43"/>
     </row>
-    <row r="26" spans="1:91" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="57" t="s">
-        <v>32</v>
-      </c>
-      <c r="B26" s="32" t="s">
-        <v>48</v>
-      </c>
-      <c r="C26" s="75"/>
-      <c r="D26" s="33"/>
-      <c r="E26" s="34"/>
-      <c r="F26" s="35"/>
+    <row r="26" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A26" s="47"/>
+      <c r="B26" s="68" t="s">
+        <v>0</v>
+      </c>
+      <c r="C26" s="65"/>
+      <c r="D26" s="36"/>
+      <c r="E26" s="58" t="s">
+        <v>16</v>
+      </c>
+      <c r="F26" s="58" t="s">
+        <v>16</v>
+      </c>
       <c r="G26" s="16"/>
-      <c r="H26" s="16" t="str">
+      <c r="H26" s="16" t="e">
         <f t="shared" si="6"/>
-        <v/>
+        <v>#VALUE!</v>
       </c>
       <c r="I26" s="43"/>
       <c r="J26" s="43"/>
@@ -3751,18 +3491,18 @@
       <c r="BK26" s="43"/>
       <c r="BL26" s="43"/>
     </row>
-    <row r="27" spans="1:91" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="57"/>
-      <c r="B27" s="80" t="s">
-        <v>3</v>
-      </c>
-      <c r="C27" s="76"/>
+    <row r="27" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A27" s="47"/>
+      <c r="B27" s="68" t="s">
+        <v>1</v>
+      </c>
+      <c r="C27" s="65"/>
       <c r="D27" s="36"/>
-      <c r="E27" s="68" t="s">
-        <v>30</v>
-      </c>
-      <c r="F27" s="68" t="s">
-        <v>30</v>
+      <c r="E27" s="58" t="s">
+        <v>16</v>
+      </c>
+      <c r="F27" s="58" t="s">
+        <v>16</v>
       </c>
       <c r="G27" s="16"/>
       <c r="H27" s="16" t="e">
@@ -3826,18 +3566,18 @@
       <c r="BK27" s="43"/>
       <c r="BL27" s="43"/>
     </row>
-    <row r="28" spans="1:91" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="57"/>
-      <c r="B28" s="80" t="s">
-        <v>4</v>
-      </c>
-      <c r="C28" s="76"/>
+    <row r="28" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A28" s="47"/>
+      <c r="B28" s="68" t="s">
+        <v>2</v>
+      </c>
+      <c r="C28" s="65"/>
       <c r="D28" s="36"/>
-      <c r="E28" s="68" t="s">
-        <v>30</v>
-      </c>
-      <c r="F28" s="68" t="s">
-        <v>30</v>
+      <c r="E28" s="58" t="s">
+        <v>16</v>
+      </c>
+      <c r="F28" s="58" t="s">
+        <v>16</v>
       </c>
       <c r="G28" s="16"/>
       <c r="H28" s="16" t="e">
@@ -3901,507 +3641,96 @@
       <c r="BK28" s="43"/>
       <c r="BL28" s="43"/>
     </row>
-    <row r="29" spans="1:91" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="57"/>
-      <c r="B29" s="80" t="s">
-        <v>0</v>
-      </c>
-      <c r="C29" s="76"/>
-      <c r="D29" s="36"/>
-      <c r="E29" s="68" t="s">
-        <v>30</v>
-      </c>
-      <c r="F29" s="68" t="s">
-        <v>30</v>
-      </c>
-      <c r="G29" s="16"/>
-      <c r="H29" s="16" t="e">
-        <f t="shared" si="6"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I29" s="43"/>
-      <c r="J29" s="43"/>
-      <c r="K29" s="43"/>
-      <c r="L29" s="43"/>
-      <c r="M29" s="43"/>
-      <c r="N29" s="43"/>
-      <c r="O29" s="43"/>
-      <c r="P29" s="43"/>
-      <c r="Q29" s="43"/>
-      <c r="R29" s="43"/>
-      <c r="S29" s="43"/>
-      <c r="T29" s="43"/>
-      <c r="U29" s="43"/>
-      <c r="V29" s="43"/>
-      <c r="W29" s="43"/>
-      <c r="X29" s="43"/>
-      <c r="Y29" s="43"/>
-      <c r="Z29" s="43"/>
-      <c r="AA29" s="43"/>
-      <c r="AB29" s="43"/>
-      <c r="AC29" s="43"/>
-      <c r="AD29" s="43"/>
-      <c r="AE29" s="43"/>
-      <c r="AF29" s="43"/>
-      <c r="AG29" s="43"/>
-      <c r="AH29" s="43"/>
-      <c r="AI29" s="43"/>
-      <c r="AJ29" s="43"/>
-      <c r="AK29" s="43"/>
-      <c r="AL29" s="43"/>
-      <c r="AM29" s="43"/>
-      <c r="AN29" s="43"/>
-      <c r="AO29" s="43"/>
-      <c r="AP29" s="43"/>
-      <c r="AQ29" s="43"/>
-      <c r="AR29" s="43"/>
-      <c r="AS29" s="43"/>
-      <c r="AT29" s="43"/>
-      <c r="AU29" s="43"/>
-      <c r="AV29" s="43"/>
-      <c r="AW29" s="43"/>
-      <c r="AX29" s="43"/>
-      <c r="AY29" s="43"/>
-      <c r="AZ29" s="43"/>
-      <c r="BA29" s="43"/>
-      <c r="BB29" s="43"/>
-      <c r="BC29" s="43"/>
-      <c r="BD29" s="43"/>
-      <c r="BE29" s="43"/>
-      <c r="BF29" s="43"/>
-      <c r="BG29" s="43"/>
-      <c r="BH29" s="43"/>
-      <c r="BI29" s="43"/>
-      <c r="BJ29" s="43"/>
-      <c r="BK29" s="43"/>
-      <c r="BL29" s="43"/>
-    </row>
-    <row r="30" spans="1:91" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A30" s="57"/>
-      <c r="B30" s="80" t="s">
-        <v>1</v>
-      </c>
-      <c r="C30" s="76"/>
-      <c r="D30" s="36"/>
-      <c r="E30" s="68" t="s">
-        <v>30</v>
-      </c>
-      <c r="F30" s="68" t="s">
-        <v>30</v>
-      </c>
-      <c r="G30" s="16"/>
-      <c r="H30" s="16" t="e">
-        <f t="shared" si="6"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I30" s="43"/>
-      <c r="J30" s="43"/>
-      <c r="K30" s="43"/>
-      <c r="L30" s="43"/>
-      <c r="M30" s="43"/>
-      <c r="N30" s="43"/>
-      <c r="O30" s="43"/>
-      <c r="P30" s="43"/>
-      <c r="Q30" s="43"/>
-      <c r="R30" s="43"/>
-      <c r="S30" s="43"/>
-      <c r="T30" s="43"/>
-      <c r="U30" s="43"/>
-      <c r="V30" s="43"/>
-      <c r="W30" s="43"/>
-      <c r="X30" s="43"/>
-      <c r="Y30" s="43"/>
-      <c r="Z30" s="43"/>
-      <c r="AA30" s="43"/>
-      <c r="AB30" s="43"/>
-      <c r="AC30" s="43"/>
-      <c r="AD30" s="43"/>
-      <c r="AE30" s="43"/>
-      <c r="AF30" s="43"/>
-      <c r="AG30" s="43"/>
-      <c r="AH30" s="43"/>
-      <c r="AI30" s="43"/>
-      <c r="AJ30" s="43"/>
-      <c r="AK30" s="43"/>
-      <c r="AL30" s="43"/>
-      <c r="AM30" s="43"/>
-      <c r="AN30" s="43"/>
-      <c r="AO30" s="43"/>
-      <c r="AP30" s="43"/>
-      <c r="AQ30" s="43"/>
-      <c r="AR30" s="43"/>
-      <c r="AS30" s="43"/>
-      <c r="AT30" s="43"/>
-      <c r="AU30" s="43"/>
-      <c r="AV30" s="43"/>
-      <c r="AW30" s="43"/>
-      <c r="AX30" s="43"/>
-      <c r="AY30" s="43"/>
-      <c r="AZ30" s="43"/>
-      <c r="BA30" s="43"/>
-      <c r="BB30" s="43"/>
-      <c r="BC30" s="43"/>
-      <c r="BD30" s="43"/>
-      <c r="BE30" s="43"/>
-      <c r="BF30" s="43"/>
-      <c r="BG30" s="43"/>
-      <c r="BH30" s="43"/>
-      <c r="BI30" s="43"/>
-      <c r="BJ30" s="43"/>
-      <c r="BK30" s="43"/>
-      <c r="BL30" s="43"/>
-    </row>
-    <row r="31" spans="1:91" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A31" s="57"/>
-      <c r="B31" s="80" t="s">
-        <v>2</v>
-      </c>
-      <c r="C31" s="76"/>
-      <c r="D31" s="36"/>
-      <c r="E31" s="68" t="s">
-        <v>30</v>
-      </c>
-      <c r="F31" s="68" t="s">
-        <v>30</v>
-      </c>
-      <c r="G31" s="16"/>
-      <c r="H31" s="16" t="e">
-        <f t="shared" si="6"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I31" s="43"/>
-      <c r="J31" s="43"/>
-      <c r="K31" s="43"/>
-      <c r="L31" s="43"/>
-      <c r="M31" s="43"/>
-      <c r="N31" s="43"/>
-      <c r="O31" s="43"/>
-      <c r="P31" s="43"/>
-      <c r="Q31" s="43"/>
-      <c r="R31" s="43"/>
-      <c r="S31" s="43"/>
-      <c r="T31" s="43"/>
-      <c r="U31" s="43"/>
-      <c r="V31" s="43"/>
-      <c r="W31" s="43"/>
-      <c r="X31" s="43"/>
-      <c r="Y31" s="43"/>
-      <c r="Z31" s="43"/>
-      <c r="AA31" s="43"/>
-      <c r="AB31" s="43"/>
-      <c r="AC31" s="43"/>
-      <c r="AD31" s="43"/>
-      <c r="AE31" s="43"/>
-      <c r="AF31" s="43"/>
-      <c r="AG31" s="43"/>
-      <c r="AH31" s="43"/>
-      <c r="AI31" s="43"/>
-      <c r="AJ31" s="43"/>
-      <c r="AK31" s="43"/>
-      <c r="AL31" s="43"/>
-      <c r="AM31" s="43"/>
-      <c r="AN31" s="43"/>
-      <c r="AO31" s="43"/>
-      <c r="AP31" s="43"/>
-      <c r="AQ31" s="43"/>
-      <c r="AR31" s="43"/>
-      <c r="AS31" s="43"/>
-      <c r="AT31" s="43"/>
-      <c r="AU31" s="43"/>
-      <c r="AV31" s="43"/>
-      <c r="AW31" s="43"/>
-      <c r="AX31" s="43"/>
-      <c r="AY31" s="43"/>
-      <c r="AZ31" s="43"/>
-      <c r="BA31" s="43"/>
-      <c r="BB31" s="43"/>
-      <c r="BC31" s="43"/>
-      <c r="BD31" s="43"/>
-      <c r="BE31" s="43"/>
-      <c r="BF31" s="43"/>
-      <c r="BG31" s="43"/>
-      <c r="BH31" s="43"/>
-      <c r="BI31" s="43"/>
-      <c r="BJ31" s="43"/>
-      <c r="BK31" s="43"/>
-      <c r="BL31" s="43"/>
-    </row>
-    <row r="32" spans="1:91" s="92" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A32" s="93"/>
-      <c r="B32" s="103" t="s">
-        <v>49</v>
-      </c>
-      <c r="C32" s="88"/>
-      <c r="D32" s="89"/>
-      <c r="E32" s="90"/>
-      <c r="F32" s="91"/>
-      <c r="G32" s="94"/>
-      <c r="H32" s="94" t="str">
+    <row r="29" spans="1:64" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A29" s="48" t="s">
+        <v>18</v>
+      </c>
+      <c r="B29" s="37" t="s">
+        <v>4</v>
+      </c>
+      <c r="C29" s="38"/>
+      <c r="D29" s="39"/>
+      <c r="E29" s="40"/>
+      <c r="F29" s="41"/>
+      <c r="G29" s="42"/>
+      <c r="H29" s="42" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="I32" s="95"/>
-      <c r="J32" s="95"/>
-      <c r="K32" s="95"/>
-      <c r="L32" s="95"/>
-      <c r="M32" s="95"/>
-      <c r="N32" s="95"/>
-      <c r="O32" s="95"/>
-      <c r="P32" s="95"/>
-      <c r="Q32" s="95"/>
-      <c r="R32" s="95"/>
-      <c r="S32" s="95"/>
-      <c r="T32" s="95"/>
-      <c r="U32" s="95"/>
-      <c r="V32" s="95"/>
-      <c r="W32" s="95"/>
-      <c r="X32" s="95"/>
-      <c r="Y32" s="95"/>
-      <c r="Z32" s="95"/>
-      <c r="AA32" s="95"/>
-      <c r="AB32" s="95"/>
-      <c r="AC32" s="95"/>
-      <c r="AD32" s="95"/>
-      <c r="AE32" s="95"/>
-      <c r="AF32" s="95"/>
-      <c r="AG32" s="95"/>
-      <c r="AH32" s="95"/>
-      <c r="AI32" s="95"/>
-      <c r="AJ32" s="95"/>
-      <c r="AK32" s="95"/>
-      <c r="AL32" s="95"/>
-      <c r="AM32" s="95"/>
-      <c r="AN32" s="95"/>
-      <c r="AO32" s="95"/>
-      <c r="AP32" s="95"/>
-      <c r="AQ32" s="95"/>
-      <c r="AR32" s="95"/>
-      <c r="AS32" s="95"/>
-      <c r="AT32" s="95"/>
-      <c r="AU32" s="95"/>
-      <c r="AV32" s="95"/>
-      <c r="AW32" s="95"/>
-      <c r="AX32" s="95"/>
-      <c r="AY32" s="95"/>
-      <c r="AZ32" s="95"/>
-      <c r="BA32" s="95"/>
-      <c r="BB32" s="95"/>
-      <c r="BC32" s="95"/>
-      <c r="BD32" s="95"/>
-      <c r="BE32" s="95"/>
-      <c r="BF32" s="95"/>
-      <c r="BG32" s="95"/>
-      <c r="BH32" s="95"/>
-      <c r="BI32" s="95"/>
-      <c r="BJ32" s="95"/>
-      <c r="BK32" s="95"/>
-      <c r="BL32" s="95"/>
-      <c r="BM32" s="96"/>
-      <c r="BN32" s="96"/>
-      <c r="BO32" s="96"/>
-      <c r="BP32" s="96"/>
-      <c r="BQ32" s="96"/>
-      <c r="BR32" s="96"/>
-      <c r="BS32" s="96"/>
-      <c r="BT32" s="96"/>
-      <c r="BU32" s="96"/>
-      <c r="BV32" s="96"/>
-      <c r="BW32" s="96"/>
-      <c r="BX32" s="96"/>
-      <c r="BY32" s="96"/>
-      <c r="BZ32" s="96"/>
-      <c r="CA32" s="96"/>
-      <c r="CB32" s="96"/>
-      <c r="CC32" s="96"/>
-      <c r="CD32" s="96"/>
-      <c r="CE32" s="96"/>
-      <c r="CF32" s="96"/>
-      <c r="CG32" s="96"/>
-      <c r="CH32" s="96"/>
-      <c r="CI32" s="96"/>
-      <c r="CJ32" s="96"/>
-      <c r="CK32" s="96"/>
-      <c r="CL32" s="96"/>
-      <c r="CM32" s="96"/>
+      <c r="I29" s="45"/>
+      <c r="J29" s="45"/>
+      <c r="K29" s="45"/>
+      <c r="L29" s="45"/>
+      <c r="M29" s="45"/>
+      <c r="N29" s="45"/>
+      <c r="O29" s="45"/>
+      <c r="P29" s="45"/>
+      <c r="Q29" s="45"/>
+      <c r="R29" s="45"/>
+      <c r="S29" s="45"/>
+      <c r="T29" s="45"/>
+      <c r="U29" s="45"/>
+      <c r="V29" s="45"/>
+      <c r="W29" s="45"/>
+      <c r="X29" s="45"/>
+      <c r="Y29" s="45"/>
+      <c r="Z29" s="45"/>
+      <c r="AA29" s="45"/>
+      <c r="AB29" s="45"/>
+      <c r="AC29" s="45"/>
+      <c r="AD29" s="45"/>
+      <c r="AE29" s="45"/>
+      <c r="AF29" s="45"/>
+      <c r="AG29" s="45"/>
+      <c r="AH29" s="45"/>
+      <c r="AI29" s="45"/>
+      <c r="AJ29" s="45"/>
+      <c r="AK29" s="45"/>
+      <c r="AL29" s="45"/>
+      <c r="AM29" s="45"/>
+      <c r="AN29" s="45"/>
+      <c r="AO29" s="45"/>
+      <c r="AP29" s="45"/>
+      <c r="AQ29" s="45"/>
+      <c r="AR29" s="45"/>
+      <c r="AS29" s="45"/>
+      <c r="AT29" s="45"/>
+      <c r="AU29" s="45"/>
+      <c r="AV29" s="45"/>
+      <c r="AW29" s="45"/>
+      <c r="AX29" s="45"/>
+      <c r="AY29" s="45"/>
+      <c r="AZ29" s="45"/>
+      <c r="BA29" s="45"/>
+      <c r="BB29" s="45"/>
+      <c r="BC29" s="45"/>
+      <c r="BD29" s="45"/>
+      <c r="BE29" s="45"/>
+      <c r="BF29" s="45"/>
+      <c r="BG29" s="45"/>
+      <c r="BH29" s="45"/>
+      <c r="BI29" s="45"/>
+      <c r="BJ29" s="45"/>
+      <c r="BK29" s="45"/>
+      <c r="BL29" s="45"/>
     </row>
-    <row r="33" spans="1:91" s="92" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A33" s="93"/>
-      <c r="B33" s="104"/>
-      <c r="C33" s="99"/>
-      <c r="D33" s="97"/>
-      <c r="E33" s="98"/>
-      <c r="F33" s="98"/>
-      <c r="G33" s="94"/>
-      <c r="H33" s="94"/>
-      <c r="I33" s="95"/>
-      <c r="J33" s="95"/>
-      <c r="K33" s="95"/>
-      <c r="L33" s="95"/>
-      <c r="M33" s="95"/>
-      <c r="N33" s="95"/>
-      <c r="O33" s="95"/>
-      <c r="P33" s="95"/>
-      <c r="Q33" s="95"/>
-      <c r="R33" s="95"/>
-      <c r="S33" s="95"/>
-      <c r="T33" s="95"/>
-      <c r="U33" s="95"/>
-      <c r="V33" s="95"/>
-      <c r="W33" s="95"/>
-      <c r="X33" s="95"/>
-      <c r="Y33" s="95"/>
-      <c r="Z33" s="95"/>
-      <c r="AA33" s="95"/>
-      <c r="AB33" s="95"/>
-      <c r="AC33" s="95"/>
-      <c r="AD33" s="95"/>
-      <c r="AE33" s="95"/>
-      <c r="AF33" s="95"/>
-      <c r="AG33" s="95"/>
-      <c r="AH33" s="95"/>
-      <c r="AI33" s="95"/>
-      <c r="AJ33" s="95"/>
-      <c r="AK33" s="95"/>
-      <c r="AL33" s="95"/>
-      <c r="AM33" s="95"/>
-      <c r="AN33" s="95"/>
-      <c r="AO33" s="95"/>
-      <c r="AP33" s="95"/>
-      <c r="AQ33" s="95"/>
-      <c r="AR33" s="95"/>
-      <c r="AS33" s="95"/>
-      <c r="AT33" s="95"/>
-      <c r="AU33" s="95"/>
-      <c r="AV33" s="95"/>
-      <c r="AW33" s="95"/>
-      <c r="AX33" s="95"/>
-      <c r="AY33" s="95"/>
-      <c r="AZ33" s="95"/>
-      <c r="BA33" s="95"/>
-      <c r="BB33" s="95"/>
-      <c r="BC33" s="95"/>
-      <c r="BD33" s="95"/>
-      <c r="BE33" s="95"/>
-      <c r="BF33" s="95"/>
-      <c r="BG33" s="95"/>
-      <c r="BH33" s="95"/>
-      <c r="BI33" s="95"/>
-      <c r="BJ33" s="95"/>
-      <c r="BK33" s="95"/>
-      <c r="BL33" s="95"/>
-      <c r="BM33" s="96"/>
-      <c r="BN33" s="96"/>
-      <c r="BO33" s="96"/>
-      <c r="BP33" s="96"/>
-      <c r="BQ33" s="96"/>
-      <c r="BR33" s="96"/>
-      <c r="BS33" s="96"/>
-      <c r="BT33" s="96"/>
-      <c r="BU33" s="96"/>
-      <c r="BV33" s="96"/>
-      <c r="BW33" s="96"/>
-      <c r="BX33" s="96"/>
-      <c r="BY33" s="96"/>
-      <c r="BZ33" s="96"/>
-      <c r="CA33" s="96"/>
-      <c r="CB33" s="96"/>
-      <c r="CC33" s="96"/>
-      <c r="CD33" s="96"/>
-      <c r="CE33" s="96"/>
-      <c r="CF33" s="96"/>
-      <c r="CG33" s="96"/>
-      <c r="CH33" s="96"/>
-      <c r="CI33" s="96"/>
-      <c r="CJ33" s="96"/>
-      <c r="CK33" s="96"/>
-      <c r="CL33" s="96"/>
-      <c r="CM33" s="96"/>
+    <row r="30" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G30" s="6"/>
     </row>
-    <row r="34" spans="1:91" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A34" s="58" t="s">
-        <v>33</v>
-      </c>
-      <c r="B34" s="37" t="s">
-        <v>5</v>
-      </c>
-      <c r="C34" s="38"/>
-      <c r="D34" s="39"/>
-      <c r="E34" s="40"/>
-      <c r="F34" s="41"/>
-      <c r="G34" s="42"/>
-      <c r="H34" s="42" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="I34" s="45"/>
-      <c r="J34" s="45"/>
-      <c r="K34" s="45"/>
-      <c r="L34" s="45"/>
-      <c r="M34" s="45"/>
-      <c r="N34" s="45"/>
-      <c r="O34" s="45"/>
-      <c r="P34" s="45"/>
-      <c r="Q34" s="45"/>
-      <c r="R34" s="45"/>
-      <c r="S34" s="45"/>
-      <c r="T34" s="45"/>
-      <c r="U34" s="45"/>
-      <c r="V34" s="45"/>
-      <c r="W34" s="45"/>
-      <c r="X34" s="45"/>
-      <c r="Y34" s="45"/>
-      <c r="Z34" s="45"/>
-      <c r="AA34" s="45"/>
-      <c r="AB34" s="45"/>
-      <c r="AC34" s="45"/>
-      <c r="AD34" s="45"/>
-      <c r="AE34" s="45"/>
-      <c r="AF34" s="45"/>
-      <c r="AG34" s="45"/>
-      <c r="AH34" s="45"/>
-      <c r="AI34" s="45"/>
-      <c r="AJ34" s="45"/>
-      <c r="AK34" s="45"/>
-      <c r="AL34" s="45"/>
-      <c r="AM34" s="45"/>
-      <c r="AN34" s="45"/>
-      <c r="AO34" s="45"/>
-      <c r="AP34" s="45"/>
-      <c r="AQ34" s="45"/>
-      <c r="AR34" s="45"/>
-      <c r="AS34" s="45"/>
-      <c r="AT34" s="45"/>
-      <c r="AU34" s="45"/>
-      <c r="AV34" s="45"/>
-      <c r="AW34" s="45"/>
-      <c r="AX34" s="45"/>
-      <c r="AY34" s="45"/>
-      <c r="AZ34" s="45"/>
-      <c r="BA34" s="45"/>
-      <c r="BB34" s="45"/>
-      <c r="BC34" s="45"/>
-      <c r="BD34" s="45"/>
-      <c r="BE34" s="45"/>
-      <c r="BF34" s="45"/>
-      <c r="BG34" s="45"/>
-      <c r="BH34" s="45"/>
-      <c r="BI34" s="45"/>
-      <c r="BJ34" s="45"/>
-      <c r="BK34" s="45"/>
-      <c r="BL34" s="45"/>
+    <row r="31" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C31" s="14"/>
+      <c r="F31" s="49"/>
     </row>
-    <row r="35" spans="1:91" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="G35" s="6"/>
-    </row>
-    <row r="36" spans="1:91" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C36" s="14"/>
-      <c r="F36" s="59"/>
-    </row>
-    <row r="37" spans="1:91" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C37" s="15"/>
+    <row r="32" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C32" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="AK4:AQ4"/>
+    <mergeCell ref="AR4:AX4"/>
     <mergeCell ref="AY4:BE4"/>
     <mergeCell ref="BF4:BL4"/>
     <mergeCell ref="E3:F3"/>
@@ -4409,13 +3738,8 @@
     <mergeCell ref="P4:V4"/>
     <mergeCell ref="W4:AC4"/>
     <mergeCell ref="AD4:AJ4"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="AK4:AQ4"/>
-    <mergeCell ref="AR4:AX4"/>
   </mergeCells>
-  <conditionalFormatting sqref="D7:D31 D34">
+  <conditionalFormatting sqref="D7:D29">
     <cfRule type="dataBar" priority="18">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -4429,43 +3753,16 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I5:BL31 I34:BL34">
-    <cfRule type="expression" dxfId="5" priority="37">
+  <conditionalFormatting sqref="I5:BL29">
+    <cfRule type="expression" dxfId="2" priority="37">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I7:BL31 I34:BL34">
-    <cfRule type="expression" dxfId="4" priority="31">
+  <conditionalFormatting sqref="I7:BL29">
+    <cfRule type="expression" dxfId="1" priority="31">
       <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="32" stopIfTrue="1">
-      <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D32:D33">
-    <cfRule type="dataBar" priority="1">
-      <dataBar>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="1"/>
-        <color theme="0" tint="-0.249977111117893"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{0E1ACEB4-4D47-4693-9C6F-81A3585E30EA}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I32:BL33">
-    <cfRule type="expression" dxfId="2" priority="4">
-      <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I32:BL33">
-    <cfRule type="expression" dxfId="1" priority="2">
-      <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="0" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="0" priority="32" stopIfTrue="1">
       <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4485,7 +3782,7 @@
     <oddFooter>Page &amp;P of &amp;N</oddFooter>
   </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="F18 F22:F23 E23" formula="1"/>
+    <ignoredError sqref="F19:F20 E20" formula="1"/>
   </ignoredErrors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
@@ -4503,128 +3800,10 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D7:D31 D34</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{0E1ACEB4-4D47-4693-9C6F-81A3585E30EA}">
-            <x14:dataBar minLength="0" maxLength="100" gradient="0">
-              <x14:cfvo type="num">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>D32:D33</xm:sqref>
+          <xm:sqref>D7:D29</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
   </extLst>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B16"/>
-  <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="87.1796875" style="47" customWidth="1"/>
-    <col min="2" max="16384" width="9.1796875" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="46.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:2" s="49" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="48" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="48"/>
-    </row>
-    <row r="3" spans="1:2" s="53" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="54" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" s="54"/>
-    </row>
-    <row r="4" spans="1:2" s="50" customFormat="1" ht="26" x14ac:dyDescent="0.6">
-      <c r="A4" s="51" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="74.150000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="52" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="51" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" s="47" customFormat="1" ht="205" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="56" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" s="50" customFormat="1" ht="26" x14ac:dyDescent="0.6">
-      <c r="A8" s="51" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="58" x14ac:dyDescent="0.3">
-      <c r="A9" s="52" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" s="47" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="55" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" s="50" customFormat="1" ht="26" x14ac:dyDescent="0.6">
-      <c r="A11" s="51" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="29" x14ac:dyDescent="0.3">
-      <c r="A12" s="52" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" s="47" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="55" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" s="50" customFormat="1" ht="26" x14ac:dyDescent="0.6">
-      <c r="A14" s="51" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="52" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="72.5" x14ac:dyDescent="0.3">
-      <c r="A16" s="52" t="s">
-        <v>21</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A13" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="A10" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
-    <hyperlink ref="A3" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
-    <hyperlink ref="A2" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
-  </hyperlinks>
-  <pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
-  <drawing r:id="rId6"/>
-</worksheet>
 </file>
</xml_diff>